<commit_message>
Added column types info
</commit_message>
<xml_diff>
--- a/data/neokruga.xlsx
+++ b/data/neokruga.xlsx
@@ -59,7 +59,7 @@
     <t xml:space="preserve">Липецкая область</t>
   </si>
   <si>
-    <t xml:space="preserve">Московская область1) </t>
+    <t xml:space="preserve">Московская область1)</t>
   </si>
   <si>
     <t xml:space="preserve">Орловская область</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">Республика Дагестан</t>
   </si>
   <si>
-    <t xml:space="preserve">Республика Ингушетия </t>
+    <t xml:space="preserve">Республика Ингушетия</t>
   </si>
   <si>
     <t xml:space="preserve">Кабардино-Балкарская Республика</t>
@@ -152,7 +152,7 @@
     <t xml:space="preserve">Республика Северная Осетия - Алания</t>
   </si>
   <si>
-    <t xml:space="preserve">Чеченская Республика </t>
+    <t xml:space="preserve">Чеченская Республика</t>
   </si>
   <si>
     <t xml:space="preserve">Республика Башкортостан</t>

</xml_diff>